<commit_message>
Add new level double floor one color
</commit_message>
<xml_diff>
--- a/BlockDisappear/docments/levelconfig.xlsx
+++ b/BlockDisappear/docments/levelconfig.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>i</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -52,9 +52,6 @@
     <t>Level-a1</t>
   </si>
   <si>
-    <t>Level-a3</t>
-  </si>
-  <si>
     <t>Level-a2</t>
   </si>
   <si>
@@ -148,6 +145,15 @@
   </si>
   <si>
     <t>Level-ct4a-4-1201-2</t>
+  </si>
+  <si>
+    <t>Level-c1-t0-1216</t>
+  </si>
+  <si>
+    <t>Level-c1-t1-1216</t>
+  </si>
+  <si>
+    <t>Level-c1-t2-1216</t>
   </si>
 </sst>
 </file>
@@ -220,17 +226,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -514,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="B3" sqref="B3:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,7 +523,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -541,7 +537,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -551,249 +547,249 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
         <v>21</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
@@ -804,97 +800,119 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
         <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
         <v>26</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
         <v>27</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
         <v>29</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
         <v>30</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
         <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>32</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C3:C33">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="C6:C35">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>